<commit_message>
Before pushing to github
</commit_message>
<xml_diff>
--- a/doc/report_example.xlsx
+++ b/doc/report_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knliao\Fall 2020\substation_readings_manager\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F488D9-330C-42E8-A76A-9BEBA669A488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82671E77-02F2-4539-B8D9-01F182390B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Substation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Malborn</t>
   </si>
@@ -37,12 +34,6 @@
     <t>Required</t>
   </si>
   <si>
-    <t xml:space="preserve">Actual </t>
-  </si>
-  <si>
-    <t>Lauderdale West</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -61,10 +52,28 @@
     <t xml:space="preserve">Strap(60) + Intertier(Varies) + Cell(60) </t>
   </si>
   <si>
-    <t xml:space="preserve">NASA </t>
-  </si>
-  <si>
-    <t>Ordering should be reds, then blues, then purple</t>
+    <t xml:space="preserve">Voltage is read every day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substation </t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Impedance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage </t>
+  </si>
+  <si>
+    <t>Lauderdale West #1</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Shubuta</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +114,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -118,11 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +422,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,31 +433,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -451,10 +470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B497ACEC-83F7-4282-AE5A-3FDDB8797C9D}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -464,39 +483,63 @@
     <col min="5" max="5" width="41.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1700</v>
+      </c>
+      <c r="C5">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1900</v>
+      </c>
+      <c r="C7">
+        <v>1930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>